<commit_message>
working identification and visual output, some more data is missing
</commit_message>
<xml_diff>
--- a/out/Frederikssund Hospital (FSH), Køkken - Økologi statistik december 2024.xlsx
+++ b/out/Frederikssund Hospital (FSH), Køkken - Økologi statistik december 2024.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="FirstPass" sheetId="2" r:id="rId6"/>
     <sheet name="SecondPass" sheetId="3" r:id="rId7"/>
+    <sheet name="ThirdPass" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>1056930 - FRISKSNIT.dk</t>
   </si>
@@ -221,6 +222,66 @@
   </si>
   <si>
     <t>STK. MASSE 2, TOTAL MASSE 2</t>
+  </si>
+  <si>
+    <t>varenavn oplyst</t>
+  </si>
+  <si>
+    <t>vare</t>
+  </si>
+  <si>
+    <t>ingrediens</t>
+  </si>
+  <si>
+    <t>kategori</t>
+  </si>
+  <si>
+    <t>Vare Nr.</t>
+  </si>
+  <si>
+    <t>Masse per styk</t>
+  </si>
+  <si>
+    <t>antal</t>
+  </si>
+  <si>
+    <t>Samlet masse</t>
+  </si>
+  <si>
+    <t>tabel</t>
+  </si>
+  <si>
+    <t>Frugtmix</t>
+  </si>
+  <si>
+    <t>frugt, blandet</t>
+  </si>
+  <si>
+    <t>frugt og bær</t>
+  </si>
+  <si>
+    <t>rødløg</t>
+  </si>
+  <si>
+    <t>løg</t>
+  </si>
+  <si>
+    <t>grøntsager</t>
+  </si>
+  <si>
+    <t>porre</t>
+  </si>
+  <si>
+    <t>DRUER</t>
+  </si>
+  <si>
+    <t>vindrue</t>
+  </si>
+  <si>
+    <t>Kartoffel</t>
+  </si>
+  <si>
+    <t>kartoffel</t>
   </si>
 </sst>
 </file>
@@ -387,35 +448,35 @@
     <xf numFmtId="0" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="3" applyFont="1" fillId="6" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="3" applyFont="1" fillId="7" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" applyFill="1" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" applyFill="1" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="11" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" applyFill="1" borderId="0"/>
     <xf numFmtId="4" applyNumberFormat="1" fontId="0" fillId="11" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" applyNumberFormat="1" fontId="0" fillId="12" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" applyFill="1" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="13" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="14" applyFill="1" borderId="0" xfId="0" applyAlignment="1">
@@ -1221,7 +1282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D0958E-9D67-45E9-875A-7BA9D66A4FA0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6F4FF0-1D15-4CEC-B6DD-DE653DAA866F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1259,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1268,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="18" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1277,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="19" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1288,16 +1349,16 @@
       <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1317,17 +1378,17 @@
       <c r="C7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="25">
-        <v>3</v>
-      </c>
-      <c r="E7" s="27">
-        <v>1</v>
-      </c>
-      <c r="F7" s="27">
+      <c r="D7" s="24">
+        <v>3</v>
+      </c>
+      <c r="E7" s="25">
+        <v>1</v>
+      </c>
+      <c r="F7" s="25">
         <f>+D7*E7</f>
         <v>3</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="26">
         <v>131.28</v>
       </c>
       <c r="H7" s="21" t="s">
@@ -1344,17 +1405,17 @@
       <c r="C8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>5</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>5</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="25">
         <f ref="F8:F14" t="shared" si="0">+D8*E8</f>
         <v>25</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="26">
         <v>893.05</v>
       </c>
       <c r="H8" s="22" t="s">
@@ -1371,20 +1432,20 @@
       <c r="C9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="25">
-        <v>1</v>
-      </c>
-      <c r="E9" s="27">
-        <v>3</v>
-      </c>
-      <c r="F9" s="27">
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25">
+        <v>3</v>
+      </c>
+      <c r="F9" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="26">
         <v>77.01</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="27" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1398,20 +1459,20 @@
       <c r="C10" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="25">
-        <v>1</v>
-      </c>
-      <c r="E10" s="27">
-        <v>3</v>
-      </c>
-      <c r="F10" s="27">
+      <c r="D10" s="24">
+        <v>1</v>
+      </c>
+      <c r="E10" s="25">
+        <v>3</v>
+      </c>
+      <c r="F10" s="25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="26">
         <v>148.17</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="28" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1428,14 +1489,14 @@
       <c r="D11" s="33">
         <v>3.2</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="25">
         <v>9</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="26">
         <f t="shared" si="0"/>
         <v>28.8</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="26">
         <v>1969.2</v>
       </c>
       <c r="H11" s="29" t="s">
@@ -1452,17 +1513,17 @@
       <c r="C12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="25">
-        <v>1</v>
-      </c>
-      <c r="E12" s="27">
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="25">
         <v>74</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="25">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="26">
         <v>4441.48</v>
       </c>
       <c r="H12" s="30" t="s">
@@ -1479,17 +1540,17 @@
       <c r="C13" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="25">
-        <v>3</v>
-      </c>
-      <c r="E13" s="27">
+      <c r="D13" s="24">
+        <v>3</v>
+      </c>
+      <c r="E13" s="25">
         <v>13</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="25">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="26">
         <v>928.72</v>
       </c>
       <c r="H13" s="32" t="s">
@@ -1506,17 +1567,17 @@
       <c r="C14" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="25">
-        <v>3</v>
-      </c>
-      <c r="E14" s="27">
+      <c r="D14" s="24">
+        <v>3</v>
+      </c>
+      <c r="E14" s="25">
         <v>4</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="25">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="26">
         <v>201.6</v>
       </c>
       <c r="H14" s="35" t="s">
@@ -1558,16 +1619,16 @@
       <c r="B17" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="16" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -1584,17 +1645,17 @@
       <c r="C18" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="25">
-        <v>3</v>
-      </c>
-      <c r="E18" s="27">
+      <c r="D18" s="24">
+        <v>3</v>
+      </c>
+      <c r="E18" s="25">
         <v>11</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="25">
         <f>+D18*E18</f>
         <v>33</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="25">
         <v>660</v>
       </c>
     </row>
@@ -1608,17 +1669,17 @@
       <c r="C19" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="25">
-        <v>3</v>
-      </c>
-      <c r="E19" s="27">
+      <c r="D19" s="24">
+        <v>3</v>
+      </c>
+      <c r="E19" s="25">
         <v>29</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="25">
         <f>+D19*E19</f>
         <v>87</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="26">
         <v>2418.75</v>
       </c>
     </row>
@@ -1693,7 +1754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1377FA84-09C0-4C11-BB0F-53C23BC3188A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B565D9C4-7ABD-47DA-96E7-F20A77895286}">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2122,6 +2183,338 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0">
+        <v>3</v>
+      </c>
+      <c r="I2" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0">
+        <v>5</v>
+      </c>
+      <c r="G3" s="0">
+        <v>5</v>
+      </c>
+      <c r="H3" s="0">
+        <v>25</v>
+      </c>
+      <c r="I3" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="0">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0">
+        <v>3</v>
+      </c>
+      <c r="H4" s="0">
+        <v>3</v>
+      </c>
+      <c r="I4" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="0">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0">
+        <v>3</v>
+      </c>
+      <c r="H5" s="0">
+        <v>3</v>
+      </c>
+      <c r="I5" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="0">
+        <v>3.2</v>
+      </c>
+      <c r="G6" s="0">
+        <v>9</v>
+      </c>
+      <c r="H6" s="0">
+        <v>28.8</v>
+      </c>
+      <c r="I6" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="0">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0">
+        <v>74</v>
+      </c>
+      <c r="H7" s="0">
+        <v>74</v>
+      </c>
+      <c r="I7" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="0">
+        <v>3</v>
+      </c>
+      <c r="G8" s="0">
+        <v>13</v>
+      </c>
+      <c r="H8" s="0">
+        <v>39</v>
+      </c>
+      <c r="I8" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="0">
+        <v>3</v>
+      </c>
+      <c r="G9" s="0">
+        <v>4</v>
+      </c>
+      <c r="H9" s="0">
+        <v>12</v>
+      </c>
+      <c r="I9" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="0">
+        <v>3</v>
+      </c>
+      <c r="G10" s="0">
+        <v>11</v>
+      </c>
+      <c r="H10" s="0">
+        <v>33</v>
+      </c>
+      <c r="I10" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="0">
+        <v>3</v>
+      </c>
+      <c r="G11" s="0">
+        <v>29</v>
+      </c>
+      <c r="H11" s="0">
+        <v>87</v>
+      </c>
+      <c r="I11" s="0">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=EPPlusLicense.txt>This workbook was created with the EPPlus library, licensed to Nikolaj R Christensen under the Polyform Noncommercial license, see https://polyformproject.org/licenses/noncommercial/1.0.0
 For more information about EPPlus, see https://epplussoftware.com/
 

</xml_diff>